<commit_message>
Graph, csv, weights saving capabilities added!
</commit_message>
<xml_diff>
--- a/transfer_learning/adjustment_log/adjustment_log.xlsx
+++ b/transfer_learning/adjustment_log/adjustment_log.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\ad-cv\transfer_learning\adjustment_log\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903061CC-E382-4140-B07C-BF8577B24D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Researched on computer vision and machine learning techniques concerning eczema classification, measurement, and monitoring. Implemented transfer learning image classifier. Image classifier achieved results of an average of about 90% and a rough 5% std. (Epochs = 1, steps_per_epoch = 22, train_batch_size = 10, val_batch size = 32, val_steps = 1. ) Also, replicated Alam et al. 2016's redness and texture measurements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restructured data set by deleting personal images and combining validation and training set into one set. Image set [207] was then split via ImageDataGenerator val_split = 0.2 to have [166] train and [41] val. Results yielded less than 50% on average with a qualitatively wide std. </t>
+  </si>
+  <si>
+    <t>10/12/2019 - 9:00AM</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 7:04PM</t>
+  </si>
+  <si>
+    <t>Added seed=7, steps_per_epoch=1, epoch=3, save fig as png, and save results to csv.</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 7:25PM</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 8:52PM</t>
+  </si>
+  <si>
+    <t>Tested 10, 20, 30 epochs and qualitatively, val_acc does not increase past 10 epochs. Val_acc &lt;= 50%. Considering addding more data aug, manually creating val and train sets, and retraining more layers.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +93,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +379,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="52.453125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43677</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>43708</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>43738</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43751</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added confusion matrix functionality!
</commit_message>
<xml_diff>
--- a/transfer_learning/adjustment_log/adjustment_log.xlsx
+++ b/transfer_learning/adjustment_log/adjustment_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Desktop\ad-cv\transfer_learning\adjustment_log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903061CC-E382-4140-B07C-BF8577B24D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F459704F-75EB-4906-977E-45E2145B57A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Start Date</t>
   </si>
@@ -57,7 +57,22 @@
     <t>10/12/2019 - 8:52PM</t>
   </si>
   <si>
-    <t>Tested 10, 20, 30 epochs and qualitatively, val_acc does not increase past 10 epochs. Val_acc &lt;= 50%. Considering addding more data aug, manually creating val and train sets, and retraining more layers.</t>
+    <t>Tested 10, 20, 30 epochs and qualitatively, val_acc does not increase past 10 epochs. Val_acc &lt;= 50%. Considering addding more data aug, manually creating val and train sets, and retraining more layers. Also, considering adding the "save best weights!"</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 10:05PM</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 10:42PM</t>
+  </si>
+  <si>
+    <t>Added "save weights" upon improvement to functionality. I would add back verbose=1 to see progress bar, or perhaps verbose=2 to see progress bar for at least the epoch. Also, debugged error: all import statements from keras must be specified tensorflow.keras...</t>
+  </si>
+  <si>
+    <t>10/12/2019 - 11:05PM</t>
+  </si>
+  <si>
+    <t>verbose=2 and save weights implemented correctly!</t>
   </si>
 </sst>
 </file>
@@ -380,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -462,6 +477,28 @@
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>